<commit_message>
able to change xlsx file metadata. Working on docx.
</commit_message>
<xml_diff>
--- a/Timesheet record CSCIL.xlsx
+++ b/Timesheet record CSCIL.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ajay Malhotra timesheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Alban Jerome timesheet" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Harkanwal Malhotra timesheet" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Baxter Wallace timesheet" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Matthew Macmillan timesheet" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Amir Mohamed timesheet" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Armeen Talwandi timesheet" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="David Hua timesheet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Dereck Tu timesheet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Derek Zhang timesheet" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Nahum Zewdie timesheet" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Mahad Khan timesheet" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ajay Malhotra timesheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Alban Jerome timesheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Harkanwal Malhotra timesheet" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Baxter Wallace timesheet" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Matthew Macmillan timesheet" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Amir Mohamed timesheet" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Armeen Talwandi timesheet" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="David Hua timesheet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dereck Tu timesheet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Derek Zhang timesheet" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nahum Zewdie timesheet" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mahad Khan timesheet" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>

</xml_diff>